<commit_message>
add summarizing data about original data in a secon sheet
</commit_message>
<xml_diff>
--- a/data/Data2.xlsx
+++ b/data/Data2.xlsx
@@ -8,13 +8,14 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="14">
   <si>
     <t>Sepal.Length</t>
   </si>
@@ -26,6 +27,30 @@
   </si>
   <si>
     <t>Petal.Width</t>
+  </si>
+  <si>
+    <t>count</t>
+  </si>
+  <si>
+    <t>mean</t>
+  </si>
+  <si>
+    <t>std</t>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>25%</t>
+  </si>
+  <si>
+    <t>50%</t>
+  </si>
+  <si>
+    <t>75%</t>
+  </si>
+  <si>
+    <t>max</t>
   </si>
   <si>
     <t>Species</t>
@@ -389,13 +414,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:5">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -408,99 +433,84 @@
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="1">
-        <v>0</v>
-      </c>
       <c r="B2">
-        <v>5.1</v>
+        <v>6</v>
       </c>
       <c r="C2">
-        <v>3.5</v>
+        <v>6</v>
       </c>
       <c r="D2">
-        <v>1.4</v>
+        <v>6</v>
       </c>
       <c r="E2">
-        <v>0.2</v>
-      </c>
-      <c r="F2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
       <c r="B3">
-        <v>4.9</v>
+        <v>4.949999999999999</v>
       </c>
       <c r="C3">
-        <v>3</v>
+        <v>3.383333333333333</v>
       </c>
       <c r="D3">
-        <v>1.4</v>
+        <v>1.45</v>
       </c>
       <c r="E3">
-        <v>0.2</v>
-      </c>
-      <c r="F3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="1">
-        <v>2</v>
+        <v>0.2333333333333333</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="B4">
-        <v>4.7</v>
+        <v>0.2880972058177588</v>
       </c>
       <c r="C4">
-        <v>3.2</v>
+        <v>0.3430257521916782</v>
       </c>
       <c r="D4">
-        <v>1.3</v>
+        <v>0.1378404875209022</v>
       </c>
       <c r="E4">
-        <v>0.2</v>
-      </c>
-      <c r="F4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="1">
-        <v>3</v>
+        <v>0.08164965809277261</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="B5">
         <v>4.6</v>
       </c>
       <c r="C5">
-        <v>3.1</v>
+        <v>3</v>
       </c>
       <c r="D5">
-        <v>1.5</v>
+        <v>1.3</v>
       </c>
       <c r="E5">
         <v>0.2</v>
       </c>
-      <c r="F5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="1">
-        <v>4</v>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="B6">
-        <v>5</v>
+        <v>4.75</v>
       </c>
       <c r="C6">
-        <v>3.6</v>
+        <v>3.125</v>
       </c>
       <c r="D6">
         <v>1.4</v>
@@ -508,28 +518,188 @@
       <c r="E6">
         <v>0.2</v>
       </c>
-      <c r="F6" t="s">
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7">
+        <v>4.95</v>
+      </c>
+      <c r="C7">
+        <v>3.35</v>
+      </c>
+      <c r="D7">
+        <v>1.4</v>
+      </c>
+      <c r="E7">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8">
+        <v>5.074999999999999</v>
+      </c>
+      <c r="C8">
+        <v>3.575</v>
+      </c>
+      <c r="D8">
+        <v>1.475</v>
+      </c>
+      <c r="E8">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9">
+        <v>5.4</v>
+      </c>
+      <c r="C9">
+        <v>3.9</v>
+      </c>
+      <c r="D9">
+        <v>1.7</v>
+      </c>
+      <c r="E9">
+        <v>0.4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2">
+        <v>5.1</v>
+      </c>
+      <c r="B2">
+        <v>3.5</v>
+      </c>
+      <c r="C2">
+        <v>1.4</v>
+      </c>
+      <c r="D2">
+        <v>0.2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3">
+        <v>4.9</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>1.4</v>
+      </c>
+      <c r="D3">
+        <v>0.2</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4">
+        <v>4.7</v>
+      </c>
+      <c r="B4">
+        <v>3.2</v>
+      </c>
+      <c r="C4">
+        <v>1.3</v>
+      </c>
+      <c r="D4">
+        <v>0.2</v>
+      </c>
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5">
+        <v>4.6</v>
+      </c>
+      <c r="B5">
+        <v>3.1</v>
+      </c>
+      <c r="C5">
+        <v>1.5</v>
+      </c>
+      <c r="D5">
+        <v>0.2</v>
+      </c>
+      <c r="E5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="1">
-        <v>5</v>
+      <c r="B6">
+        <v>3.6</v>
+      </c>
+      <c r="C6">
+        <v>1.4</v>
+      </c>
+      <c r="D6">
+        <v>0.2</v>
+      </c>
+      <c r="E6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7">
+        <v>5.4</v>
       </c>
       <c r="B7">
-        <v>5.4</v>
+        <v>3.9</v>
       </c>
       <c r="C7">
-        <v>3.9</v>
+        <v>1.7</v>
       </c>
       <c r="D7">
-        <v>1.7</v>
-      </c>
-      <c r="E7">
         <v>0.4</v>
       </c>
-      <c r="F7" t="s">
-        <v>5</v>
+      <c r="E7" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>